<commit_message>
enhanced the view stock
</commit_message>
<xml_diff>
--- a/data_stocks_pure.xlsx
+++ b/data_stocks_pure.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28012"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS57\Streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988211B4-57AF-4365-A7CC-2F471C620E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{988211B4-57AF-4365-A7CC-2F471C620E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2A7880D-FA89-467F-A8E3-A0C30BDAAD25}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{107189A6-42CD-4878-9FC7-20C8332D58C6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{107189A6-42CD-4878-9FC7-20C8332D58C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock_Price" sheetId="1" r:id="rId1"/>
-    <sheet name="Database_Stock" sheetId="2" r:id="rId2"/>
-    <sheet name="Database_Dividen" sheetId="3" r:id="rId3"/>
-    <sheet name="Database_Fund" sheetId="4" r:id="rId4"/>
+    <sheet name="Profit_Trend" sheetId="5" r:id="rId2"/>
+    <sheet name="Database_Stock" sheetId="2" r:id="rId3"/>
+    <sheet name="Database_Dividen" sheetId="3" r:id="rId4"/>
+    <sheet name="Database_Fund" sheetId="4" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="105">
+  <si>
+    <t>股票代碼</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票名稱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票中文名稱</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>2146.JP</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -292,6 +305,25 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
+    <t>日期</t>
+  </si>
+  <si>
+    <t>實際總成本</t>
+  </si>
+  <si>
+    <t>市值估算</t>
+  </si>
+  <si>
+    <t>未實現損益估算</t>
+  </si>
+  <si>
+    <t>投資報酬率</t>
+  </si>
+  <si>
+    <t>公司名</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>成交股數</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -422,36 +454,18 @@
   <si>
     <t>IE00B5649C52</t>
     <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>股票代碼</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>股票名稱</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>股票中文名稱</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>公司名</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="#,##0_);[Red]\(#,##0\)"/>
-    <numFmt numFmtId="180" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -509,6 +523,14 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -564,14 +586,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -587,16 +609,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -605,10 +627,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="38" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -617,19 +639,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -638,14 +660,32 @@
     <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="40" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="千分位" xfId="1" builtinId="3"/>
-    <cellStyle name="百分比" xfId="2" builtinId="5"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
@@ -1181,30 +1221,30 @@
   <dimension ref="A1:BF22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="58" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="58" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3">
         <v>45518</v>
@@ -1370,15 +1410,15 @@
         <v>45443</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2" s="6">
         <v>2737</v>
@@ -1535,15 +1575,15 @@
       <c r="BE2" s="8"/>
       <c r="BF2" s="8"/>
     </row>
-    <row r="3" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6">
         <v>2046.5</v>
@@ -1712,15 +1752,15 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="4" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D4" s="6">
         <v>4141</v>
@@ -1889,15 +1929,15 @@
         <v>4452</v>
       </c>
     </row>
-    <row r="5" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A5" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6">
         <v>1695.5</v>
@@ -2066,15 +2106,15 @@
         <v>1548.5</v>
       </c>
     </row>
-    <row r="6" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" s="6">
         <v>2539</v>
@@ -2243,15 +2283,15 @@
         <v>2503</v>
       </c>
     </row>
-    <row r="7" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A7" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7" s="6">
         <v>2072</v>
@@ -2374,15 +2414,15 @@
       <c r="BE7" s="8"/>
       <c r="BF7" s="8"/>
     </row>
-    <row r="8" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A8" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D8" s="6">
         <v>3234</v>
@@ -2551,15 +2591,15 @@
         <v>3432</v>
       </c>
     </row>
-    <row r="9" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A9" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D9" s="6">
         <v>4100</v>
@@ -2728,15 +2768,15 @@
         <v>4597</v>
       </c>
     </row>
-    <row r="10" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D10" s="6">
         <v>1546.5</v>
@@ -2895,15 +2935,15 @@
       <c r="BE10" s="8"/>
       <c r="BF10" s="8"/>
     </row>
-    <row r="11" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A11" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D11" s="6">
         <v>2489.5</v>
@@ -3072,15 +3112,15 @@
         <v>2473.5</v>
       </c>
     </row>
-    <row r="12" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A12" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" s="6">
         <v>2439</v>
@@ -3249,15 +3289,15 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="13" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D13" s="6">
         <v>3031</v>
@@ -3426,15 +3466,15 @@
         <v>7970</v>
       </c>
     </row>
-    <row r="14" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A14" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D14" s="6">
         <v>3378</v>
@@ -3593,15 +3633,15 @@
       <c r="BE14" s="8"/>
       <c r="BF14" s="8"/>
     </row>
-    <row r="15" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A15" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D15" s="6">
         <v>2325</v>
@@ -3758,15 +3798,15 @@
       <c r="BE15" s="8"/>
       <c r="BF15" s="8"/>
     </row>
-    <row r="16" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A16" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D16" s="6">
         <v>9699</v>
@@ -3935,15 +3975,15 @@
         <v>10290</v>
       </c>
     </row>
-    <row r="17" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A17" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D17" s="6">
         <v>4030</v>
@@ -4100,15 +4140,15 @@
       <c r="BE17" s="8"/>
       <c r="BF17" s="8"/>
     </row>
-    <row r="18" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A18" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D18" s="6">
         <v>4034</v>
@@ -4277,15 +4317,15 @@
         <v>4207</v>
       </c>
     </row>
-    <row r="19" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A19" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D19" s="6">
         <v>2338</v>
@@ -4454,15 +4494,15 @@
         <v>2639.5</v>
       </c>
     </row>
-    <row r="20" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A20" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D20" s="6">
         <v>149.30000000000001</v>
@@ -4631,15 +4671,15 @@
         <v>154.30000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A21" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D21" s="6">
         <v>4578</v>
@@ -4798,15 +4838,15 @@
       <c r="BE21" s="8"/>
       <c r="BF21" s="8"/>
     </row>
-    <row r="22" spans="1:58" s="4" customFormat="1" ht="13.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:58" s="4" customFormat="1" ht="13.5">
       <c r="A22" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D22" s="6">
         <v>5019</v>
@@ -4982,79 +5022,570 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E97B2E-0865-4C7C-B33E-9D4D0BE0861A}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="23">
+        <v>45481</v>
+      </c>
+      <c r="B2" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C2" s="24">
+        <v>5923647096</v>
+      </c>
+      <c r="D2" s="24">
+        <v>275620632</v>
+      </c>
+      <c r="E2" s="25">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="23">
+        <v>45482</v>
+      </c>
+      <c r="B3" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C3" s="24">
+        <v>5940798316</v>
+      </c>
+      <c r="D3" s="24">
+        <v>292771852</v>
+      </c>
+      <c r="E3" s="25">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="23">
+        <v>45483</v>
+      </c>
+      <c r="B4" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C4" s="24">
+        <v>5948747914</v>
+      </c>
+      <c r="D4" s="24">
+        <v>300721450</v>
+      </c>
+      <c r="E4" s="25">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="23">
+        <v>45484</v>
+      </c>
+      <c r="B5" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C5" s="24">
+        <v>5993665773</v>
+      </c>
+      <c r="D5" s="24">
+        <v>345639309</v>
+      </c>
+      <c r="E5" s="25">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="23">
+        <v>45485</v>
+      </c>
+      <c r="B6" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C6" s="24">
+        <v>5942880677</v>
+      </c>
+      <c r="D6" s="24">
+        <v>294854213</v>
+      </c>
+      <c r="E6" s="25">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="23">
+        <v>45489</v>
+      </c>
+      <c r="B7" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C7" s="24">
+        <v>5955463207</v>
+      </c>
+      <c r="D7" s="24">
+        <v>307436743</v>
+      </c>
+      <c r="E7" s="25">
+        <v>5.3999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="23">
+        <v>45490</v>
+      </c>
+      <c r="B8" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C8" s="24">
+        <v>6021284532</v>
+      </c>
+      <c r="D8" s="24">
+        <v>373258068</v>
+      </c>
+      <c r="E8" s="25">
+        <v>6.6000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="23">
+        <v>45491</v>
+      </c>
+      <c r="B9" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C9" s="24">
+        <v>6009610832</v>
+      </c>
+      <c r="D9" s="24">
+        <v>361584368</v>
+      </c>
+      <c r="E9" s="25">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="23">
+        <v>45492</v>
+      </c>
+      <c r="B10" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C10" s="24">
+        <v>5983878986</v>
+      </c>
+      <c r="D10" s="24">
+        <v>335852522</v>
+      </c>
+      <c r="E10" s="25">
+        <v>5.8999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="23">
+        <v>45495</v>
+      </c>
+      <c r="B11" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C11" s="24">
+        <v>5961682280</v>
+      </c>
+      <c r="D11" s="24">
+        <v>313655816</v>
+      </c>
+      <c r="E11" s="25">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="23">
+        <v>45496</v>
+      </c>
+      <c r="B12" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C12" s="24">
+        <v>5971365741</v>
+      </c>
+      <c r="D12" s="24">
+        <v>323339277</v>
+      </c>
+      <c r="E12" s="25">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="23">
+        <v>45497</v>
+      </c>
+      <c r="B13" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C13" s="24">
+        <v>5859154711</v>
+      </c>
+      <c r="D13" s="24">
+        <v>211128247</v>
+      </c>
+      <c r="E13" s="25">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="23">
+        <v>45498</v>
+      </c>
+      <c r="B14" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C14" s="24">
+        <v>5759191572</v>
+      </c>
+      <c r="D14" s="24">
+        <v>111165108</v>
+      </c>
+      <c r="E14" s="25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="23">
+        <v>45499</v>
+      </c>
+      <c r="B15" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C15" s="24">
+        <v>5754027488</v>
+      </c>
+      <c r="D15" s="24">
+        <v>106001024</v>
+      </c>
+      <c r="E15" s="25">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="23">
+        <v>45502</v>
+      </c>
+      <c r="B16" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C16" s="24">
+        <v>5826513052</v>
+      </c>
+      <c r="D16" s="24">
+        <v>178486588</v>
+      </c>
+      <c r="E16" s="25">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="23">
+        <v>45503</v>
+      </c>
+      <c r="B17" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C17" s="24">
+        <v>5780312119</v>
+      </c>
+      <c r="D17" s="24">
+        <v>132285655</v>
+      </c>
+      <c r="E17" s="25">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="23">
+        <v>45504</v>
+      </c>
+      <c r="B18" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C18" s="24">
+        <v>5831536057</v>
+      </c>
+      <c r="D18" s="24">
+        <v>183509593</v>
+      </c>
+      <c r="E18" s="25">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="23">
+        <v>45505</v>
+      </c>
+      <c r="B19" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C19" s="24">
+        <v>5606545320</v>
+      </c>
+      <c r="D19" s="26">
+        <v>-41481144</v>
+      </c>
+      <c r="E19" s="27">
+        <v>-7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="23">
+        <v>45506</v>
+      </c>
+      <c r="B20" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C20" s="24">
+        <v>5393749511</v>
+      </c>
+      <c r="D20" s="26">
+        <v>-254276953</v>
+      </c>
+      <c r="E20" s="27">
+        <v>-4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="23">
+        <v>45509</v>
+      </c>
+      <c r="B21" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C21" s="24">
+        <v>4796772834</v>
+      </c>
+      <c r="D21" s="26">
+        <v>-851253630</v>
+      </c>
+      <c r="E21" s="28">
+        <v>-0.151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="23">
+        <v>45510</v>
+      </c>
+      <c r="B22" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C22" s="24">
+        <v>5083377567</v>
+      </c>
+      <c r="D22" s="26">
+        <v>-564648897</v>
+      </c>
+      <c r="E22" s="28">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="23">
+        <v>45511</v>
+      </c>
+      <c r="B23" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C23" s="24">
+        <v>5239121554</v>
+      </c>
+      <c r="D23" s="26">
+        <v>-408904910</v>
+      </c>
+      <c r="E23" s="28">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="23">
+        <v>45512</v>
+      </c>
+      <c r="B24" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C24" s="24">
+        <v>5189819042</v>
+      </c>
+      <c r="D24" s="26">
+        <v>-458207422</v>
+      </c>
+      <c r="E24" s="28">
+        <v>-8.1000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="23">
+        <v>45513</v>
+      </c>
+      <c r="B25" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C25" s="24">
+        <v>5223293505</v>
+      </c>
+      <c r="D25" s="26">
+        <v>-424732959</v>
+      </c>
+      <c r="E25" s="28">
+        <v>-7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="23">
+        <v>45517</v>
+      </c>
+      <c r="B26" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C26" s="24">
+        <v>5306905954</v>
+      </c>
+      <c r="D26" s="26">
+        <v>-341120510</v>
+      </c>
+      <c r="E26" s="28">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="23">
+        <v>45518</v>
+      </c>
+      <c r="B27" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C27" s="24">
+        <v>5378074054</v>
+      </c>
+      <c r="D27" s="26">
+        <v>-269952410</v>
+      </c>
+      <c r="E27" s="28">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="23">
+        <v>45519</v>
+      </c>
+      <c r="B28" s="24">
+        <v>5648026464</v>
+      </c>
+      <c r="C28" s="24">
+        <v>5439499949</v>
+      </c>
+      <c r="D28" s="26">
+        <v>-208526515</v>
+      </c>
+      <c r="E28" s="28">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED21FA01-1509-4914-A374-CA11CEB1DA87}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L16" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" customWidth="1"/>
+    <col min="11" max="11" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="str">
         <f>VLOOKUP(A2,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>UT Group Co Ltd</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E2" s="11">
         <v>17200</v>
@@ -5085,19 +5616,19 @@
         <v>-2386128.0809600055</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5" t="str">
         <f>VLOOKUP(A3,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Kirin Holdings Co Ltd</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E3" s="11">
         <v>28000</v>
@@ -5128,19 +5659,19 @@
         <v>-6385120</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5" t="str">
         <f>VLOOKUP(A4,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Kirin Holdings Co Ltd</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E4" s="11">
         <v>94100</v>
@@ -5171,19 +5702,19 @@
         <v>-6862282.9865599871</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5" t="str">
         <f>VLOOKUP(A5,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Kirin Holdings Co Ltd</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E5" s="11">
         <v>130000</v>
@@ -5214,19 +5745,19 @@
         <v>-8095463.5539999604</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5" t="str">
         <f>VLOOKUP(A6,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Kirin Holdings Co Ltd</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E6" s="11">
         <v>185700</v>
@@ -5257,19 +5788,19 @@
         <v>-31337195.646719992</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5" t="str">
         <f>VLOOKUP(A7,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Japan Tobacco Inc</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E7" s="11">
         <v>15000</v>
@@ -5300,19 +5831,19 @@
         <v>-4317600</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5" t="str">
         <f>VLOOKUP(A8,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Japan Tobacco Inc</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E8" s="11">
         <v>11000</v>
@@ -5343,19 +5874,19 @@
         <v>-4078611.4005999938</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="str">
         <f>VLOOKUP(A9,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Japan Tobacco Inc</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E9" s="11">
         <v>52400</v>
@@ -5386,19 +5917,19 @@
         <v>-15775466.19531998</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="str">
         <f>VLOOKUP(A10,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Japan Tobacco Inc</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E10" s="11">
         <v>90400</v>
@@ -5429,19 +5960,19 @@
         <v>-36979053.068359971</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" s="5" t="str">
         <f>VLOOKUP(A11,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Astellas Pharma Inc</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E11" s="11">
         <v>53110</v>
@@ -5472,19 +6003,19 @@
         <v>-9950052.2800000012</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B12" s="5" t="str">
         <f>VLOOKUP(A12,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>H.U. Group Holdings Inc</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E12" s="11">
         <v>400</v>
@@ -5515,19 +6046,19 @@
         <v>-2339</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B13" s="5" t="str">
         <f>VLOOKUP(A13,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Toyo Tire Corp</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E13" s="11">
         <v>58300</v>
@@ -5558,19 +6089,19 @@
         <v>-28818941.892159969</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5" t="str">
         <f>VLOOKUP(A14,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Nippon Steel Corp</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E14" s="11">
         <v>12500</v>
@@ -5601,19 +6132,19 @@
         <v>213136.79999999702</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B15" s="5" t="str">
         <f>VLOOKUP(A15,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Nippon Steel Corp</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E15" s="11">
         <v>53398</v>
@@ -5644,19 +6175,19 @@
         <v>-11846251.820782661</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="str">
         <f>VLOOKUP(A16,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Komatsu Ltd</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E16" s="11">
         <v>13800</v>
@@ -5687,19 +6218,19 @@
         <v>3260774.3999999985</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5" t="str">
         <f>VLOOKUP(A17,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Komatsu Ltd</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E17" s="11">
         <v>53800</v>
@@ -5730,19 +6261,19 @@
         <v>-28305645.455439985</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B18" s="5" t="str">
         <f>VLOOKUP(A18,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Komatsu Ltd</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E18" s="11">
         <v>75800</v>
@@ -5773,19 +6304,19 @@
         <v>-38101695.329360008</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5" t="str">
         <f>VLOOKUP(A19,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Honda Motor Co Ltd</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E19" s="11">
         <v>206300</v>
@@ -5816,19 +6347,19 @@
         <v>-31190779.620599985</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A20" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B20" s="5" t="str">
         <f>VLOOKUP(A20,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Olympus Corp</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E20" s="11">
         <v>20200</v>
@@ -5859,19 +6390,19 @@
         <v>5338140.2807200029</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B21" s="5" t="str">
         <f>VLOOKUP(A21,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Marubeni Corp</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E21" s="11">
         <v>21700</v>
@@ -5902,19 +6433,19 @@
         <v>2299397.9593199939</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B22" s="5" t="str">
         <f>VLOOKUP(A22,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Marubeni Corp</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E22" s="11">
         <v>21300</v>
@@ -5945,19 +6476,19 @@
         <v>2009016</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B23" s="5" t="str">
         <f>VLOOKUP(A23,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Marubeni Corp</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E23" s="11">
         <v>35000</v>
@@ -5988,19 +6519,19 @@
         <v>6102791.498999998</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B24" s="5" t="str">
         <f>VLOOKUP(A24,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Mitsui &amp; Co Ltd</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E24" s="11">
         <v>18400</v>
@@ -6031,19 +6562,19 @@
         <v>5806672</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B25" s="5" t="str">
         <f>VLOOKUP(A25,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Mitsui &amp; Co Ltd</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E25" s="11">
         <v>17800</v>
@@ -6074,19 +6605,19 @@
         <v>5974637.0597200021</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B26" s="5" t="str">
         <f>VLOOKUP(A26,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Mitsui &amp; Co Ltd</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E26" s="11">
         <v>18400</v>
@@ -6117,19 +6648,19 @@
         <v>5747854.9206399992</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B27" s="5" t="str">
         <f>VLOOKUP(A27,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Sumitomo Corp</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E27" s="11">
         <v>12899</v>
@@ -6160,19 +6691,19 @@
         <v>-6915883.961561203</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B28" s="5" t="str">
         <f>VLOOKUP(A28,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Sumitomo Corp</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E28" s="11">
         <v>24100</v>
@@ -6203,19 +6734,19 @@
         <v>-17920452.026099995</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A29" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B29" s="5" t="str">
         <f>VLOOKUP(A29,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Sumitomo Corp</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E29" s="11">
         <v>77400</v>
@@ -6246,19 +6777,19 @@
         <v>-52598459.503800035</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B30" s="5" t="str">
         <f>VLOOKUP(A30,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Marui Group Co Ltd</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E30" s="11">
         <v>56600</v>
@@ -6289,19 +6820,19 @@
         <v>4281003.6870000064</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B31" s="5" t="str">
         <f>VLOOKUP(A31,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Marui Group Co Ltd</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E31" s="11">
         <v>106600</v>
@@ -6332,19 +6863,19 @@
         <v>-2217939.3534600139</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A32" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B32" s="5" t="str">
         <f>VLOOKUP(A32,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Sumitomo Mitsui Financial Grou</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E32" s="11">
         <v>6700</v>
@@ -6375,19 +6906,19 @@
         <v>15975480</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B33" s="5" t="str">
         <f>VLOOKUP(A33,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Sumitomo Mitsui Financial Grou</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E33" s="11">
         <v>6700</v>
@@ -6418,19 +6949,19 @@
         <v>15740511</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A34" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B34" s="5" t="str">
         <f>VLOOKUP(A34,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Sumitomo Mitsui Financial Grou</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E34" s="11">
         <v>6900</v>
@@ -6461,19 +6992,19 @@
         <v>27419650.830060005</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B35" s="5" t="str">
         <f>VLOOKUP(A35,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Jaccs Co Ltd</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E35" s="11">
         <v>10200</v>
@@ -6504,19 +7035,19 @@
         <v>-8338356.3292800039</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A36" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B36" s="5" t="str">
         <f>VLOOKUP(A36,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Dai-ichi Life Holdings Inc</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E36" s="11">
         <v>15600</v>
@@ -6547,19 +7078,19 @@
         <v>22706138.853599995</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B37" s="5" t="str">
         <f>VLOOKUP(A37,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Mitsubishi Estate Co Ltd</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E37" s="11">
         <v>25000</v>
@@ -6590,19 +7121,19 @@
         <v>17541709.2751</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A38" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B38" s="5" t="str">
         <f>VLOOKUP(A38,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Nippon Telegraph &amp; Telephone C</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E38" s="11">
         <v>1582100</v>
@@ -6633,19 +7164,19 @@
         <v>-13713334.290499955</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B39" s="5" t="str">
         <f>VLOOKUP(A39,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Nippon Telegraph &amp; Telephone C</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E39" s="11">
         <v>760000</v>
@@ -6676,19 +7207,19 @@
         <v>-3806079.9999999851</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A40" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B40" s="5" t="str">
         <f>VLOOKUP(A40,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Nippon Telegraph &amp; Telephone C</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E40" s="11">
         <v>1005700</v>
@@ -6719,19 +7250,19 @@
         <v>390457.11074000597</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B41" s="5" t="str">
         <f>VLOOKUP(A41,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>KDDI Corp</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E41" s="11">
         <v>10100</v>
@@ -6762,19 +7293,19 @@
         <v>2924176.892459996</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A42" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B42" s="5" t="str">
         <f>VLOOKUP(A42,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>KDDI Corp</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E42" s="11">
         <v>81500</v>
@@ -6805,19 +7336,19 @@
         <v>23422073.10402</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:12" s="4" customFormat="1" ht="16.5" customHeight="1">
       <c r="A43" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B43" s="5" t="str">
         <f>VLOOKUP(A43,[1]Stock_Price!$A$1:$B$22, 2, FALSE)</f>
         <v>Japan Airport Terminal Co., Ltd.</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E43" s="11">
         <v>3000</v>
@@ -6854,7 +7385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8D32AA-2103-4A94-B186-E0215CD2CB5A}">
   <dimension ref="A1:F70"/>
   <sheetViews>
@@ -6862,1410 +7393,1410 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="F2" s="5">
         <v>931500</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="F3" s="5">
         <v>500000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="F4" s="5">
         <v>75000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F5" s="5">
         <v>3340550</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F6" s="5">
         <v>397600</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F7" s="5">
         <v>994000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F8" s="5">
         <v>6592350</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6">
       <c r="A9" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F9" s="5">
         <v>1067000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F10" s="5">
         <v>601400</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F11" s="5">
         <v>1455000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6">
       <c r="A12" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F12" s="5">
         <v>8768800</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6">
       <c r="A13" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F13" s="5">
         <v>1858850</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F14" s="5">
         <v>25200</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6">
       <c r="A15" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F15" s="5">
         <v>1000000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F16" s="5">
         <v>1311000</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F17" s="5">
         <v>1292000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6">
       <c r="A18" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F18" s="5">
         <v>363600</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F19" s="5">
         <v>943950</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6">
       <c r="A20" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F20" s="5">
         <v>926550</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6">
       <c r="A21" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F21" s="5">
         <v>1522500</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F22" s="5">
         <v>391000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6">
       <c r="A23" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F23" s="5">
         <v>391000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6">
       <c r="A24" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F24" s="5">
         <v>378250</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6">
       <c r="A25" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F25" s="5">
         <v>904500</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6">
       <c r="A26" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F26" s="5">
         <v>904500</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6">
       <c r="A27" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F27" s="5">
         <v>931500</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6">
       <c r="A28" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F28" s="5">
         <v>1762800</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6">
       <c r="A29" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F29" s="5">
         <v>500000</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6">
       <c r="A30" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F30" s="5">
         <v>111000</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6">
       <c r="A31" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F31" s="5">
         <v>3340550</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6">
       <c r="A32" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F32" s="5">
         <v>4615000</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:6">
       <c r="A33" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F33" s="5">
         <v>994000</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:6">
       <c r="A34" s="5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F34" s="5">
         <v>6592350</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:6">
       <c r="A35" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F35" s="5">
         <v>1067000</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:6">
       <c r="A36" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F36" s="5">
         <v>5082800</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6">
       <c r="A37" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F37" s="5">
         <v>1455000</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:6">
       <c r="A38" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F38" s="5">
         <v>8768800</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:6">
       <c r="A39" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F39" s="5">
         <v>1965070</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:6">
       <c r="A40" s="5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F40" s="5">
         <v>24800</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6">
       <c r="A41" s="5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F41" s="5">
         <v>3206500</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:6">
       <c r="A42" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F42" s="5">
         <v>4271840</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:6">
       <c r="A43" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F43" s="5">
         <v>1000000</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6">
       <c r="A44" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F44" s="5">
         <v>1145400</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:6">
       <c r="A45" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F45" s="5">
         <v>4465400</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:6">
       <c r="A46" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F46" s="5">
         <v>6291400</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:6">
       <c r="A47" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F47" s="5">
         <v>7014200</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:6">
       <c r="A48" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F48" s="5">
         <v>976500</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:6">
       <c r="A49" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F49" s="5">
         <v>958500</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:6">
       <c r="A50" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F50" s="5">
         <v>1575000</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:6">
       <c r="A51" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F51" s="5">
         <v>920000</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:6">
       <c r="A52" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F52" s="5">
         <v>920000</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:6">
       <c r="A53" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F53" s="5">
         <v>890000</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:6">
       <c r="A54" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F54" s="5">
         <v>838435</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:6">
       <c r="A55" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F55" s="5">
         <v>1566500</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:6">
       <c r="A56" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F56" s="5">
         <v>5031000</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:6">
       <c r="A57" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F57" s="5">
         <v>2999800</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:6">
       <c r="A58" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F58" s="5">
         <v>5649800</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:6">
       <c r="A59" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F59" s="5">
         <v>1105500</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:6">
       <c r="A60" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F60" s="5">
         <v>1105500</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:6">
       <c r="A61" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F61" s="5">
         <v>1138500</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:6">
       <c r="A62" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F62" s="5">
         <v>918000</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:6">
       <c r="A63" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F63" s="5">
         <v>951600</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:6">
       <c r="A64" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F64" s="5">
         <v>525000</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:6">
       <c r="A65" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F65" s="5">
         <v>2614820</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:6">
       <c r="A66" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F66" s="5">
         <v>4113460</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:6">
       <c r="A67" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F67" s="5">
         <v>1976000</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:6">
       <c r="A68" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F68" s="5">
         <v>707000</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:6">
       <c r="A69" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F69" s="5">
         <v>5705000</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:6">
       <c r="A70" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F70" s="5">
         <v>93000</v>
@@ -8277,7 +8808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64ACD81B-CBA6-415E-AC31-3705ED6409B8}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -8285,57 +8816,57 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.08984375" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="21.125" defaultRowHeight="17.100000000000001"/>
   <cols>
-    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.75" customWidth="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9">
       <c r="A1" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>90</v>
-      </c>
       <c r="G1" s="21" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="26" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="26.1">
       <c r="A2" s="13" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D2" s="15">
         <v>11623.69</v>
@@ -8357,15 +8888,15 @@
         <v>33323</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="26.1">
       <c r="A3" s="13" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D3" s="15">
         <v>4671.1000000000004</v>
@@ -8388,15 +8919,15 @@
         <v>33323</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="26.1">
       <c r="A4" s="13" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D4" s="15">
         <v>4680.92</v>
@@ -8419,15 +8950,15 @@
         <v>33323</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="26.1">
       <c r="A5" s="13" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D5" s="15">
         <v>3089.1849999999999</v>
@@ -8457,6 +8988,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F87723316495E540ADF48B4602179522" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d22b17d56c6552e7a34e4c9784d3e34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a18b5801-1ff2-4681-81e9-5689cf63188e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="38e5821cfac28f0eada9dbc3e81d5307" ns2:_="">
     <xsd:import namespace="a18b5801-1ff2-4681-81e9-5689cf63188e"/>
@@ -8600,23 +9146,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC6647E6-C3BC-4AF3-A427-B4C72D92B05C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E08D704A-BEFF-4E8C-B5BB-B6DD22D991B6}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8624,5 +9155,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E08D704A-BEFF-4E8C-B5BB-B6DD22D991B6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC6647E6-C3BC-4AF3-A427-B4C72D92B05C}"/>
 </file>
</xml_diff>